<commit_message>
Added ability to freeze top panes
</commit_message>
<xml_diff>
--- a/writing/data/testIndex.xlsx
+++ b/writing/data/testIndex.xlsx
@@ -345,7 +345,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -382,7 +385,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+    </sheetView>
   </sheetViews>
   <sheetData>
     <row r="1">

</xml_diff>